<commit_message>
[Chore]: Converted student spreadsheet to json and included placeholder profile image
</commit_message>
<xml_diff>
--- a/src/data/student_list.xlsx
+++ b/src/data/student_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Documents\projects\niqs_dash\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DC4761E-E01C-4844-8A1C-164C5338124F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FFFCDB7A-D41D-41D0-B825-E7F31E68F7E9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="4920" xr2:uid="{8492CE45-5A31-4586-AFD1-0C964C4306C1}"/>
   </bookViews>
@@ -702,9 +702,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>reg-num</t>
-  </si>
-  <si>
     <t>QTS/2018/099</t>
   </si>
   <si>
@@ -754,6 +751,9 @@
   </si>
   <si>
     <t>QTS/2018/103</t>
+  </si>
+  <si>
+    <t>reg</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1109,7 @@
   <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,7 +1127,7 @@
         <v>224</v>
       </c>
       <c r="C1" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2271,7 +2271,7 @@
         <v>218</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2282,7 +2282,7 @@
         <v>209</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2293,7 +2293,7 @@
         <v>215</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -2304,7 +2304,7 @@
         <v>208</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -2315,7 +2315,7 @@
         <v>219</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -2326,7 +2326,7 @@
         <v>206</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -2337,7 +2337,7 @@
         <v>207</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -2348,7 +2348,7 @@
         <v>217</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -2359,7 +2359,7 @@
         <v>213</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -2370,7 +2370,7 @@
         <v>222</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -2381,7 +2381,7 @@
         <v>212</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -2392,7 +2392,7 @@
         <v>214</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -2403,7 +2403,7 @@
         <v>211</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -2414,7 +2414,7 @@
         <v>210</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -2425,7 +2425,7 @@
         <v>221</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -2436,7 +2436,7 @@
         <v>220</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -2447,7 +2447,7 @@
         <v>216</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>